<commit_message>
Revert "documentation clarification implementation"
This reverts commit 9cb038d150c457020246ca4079f51af096860d5a.

Accidental add -A
</commit_message>
<xml_diff>
--- a/Developer Notes/OMEObject Heirarchy 07052016.xlsx
+++ b/Developer Notes/OMEObject Heirarchy 07052016.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vpredovi\Desktop\JOeME\OME_live\OME\Developer Notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PWingo\Desktop\GitHub\OME\Developer Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -227,6 +227,9 @@
     <t>NullCloud</t>
   </si>
   <si>
+    <t>Represents a source/sink in Simile; this is not needed in OME since A null source/target for a Flow is effectively the same thing.</t>
+  </si>
+  <si>
     <t>NullFunc</t>
   </si>
   <si>
@@ -294,9 +297,6 @@
   </si>
   <si>
     <t>Variable which stores N dimensions of values. Fully implemented for Simile, but Vensim and XMILE equivalents have yet to be mapped.</t>
-  </si>
-  <si>
-    <t>Represents a source/sink in Simile; this is not needed in OME since a null source/target for a Flow is effectively the same thing.</t>
   </si>
 </sst>
 </file>
@@ -384,7 +384,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -402,6 +422,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -736,8 +766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:M64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,7 +1083,7 @@
         <v>54</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>55</v>
@@ -1130,7 +1160,7 @@
         <v>17</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D44" s="9" t="s">
         <v>18</v>
@@ -1139,18 +1169,18 @@
         <v>18</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D45" s="9" t="s">
         <v>18</v>
@@ -1159,18 +1189,18 @@
         <v>18</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>32</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D46" s="9" t="s">
         <v>18</v>
@@ -1179,18 +1209,18 @@
         <v>18</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>50</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D47" s="9" t="s">
         <v>18</v>
@@ -1199,12 +1229,12 @@
         <v>18</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B48" s="6" t="s">
         <v>50</v>
@@ -1213,24 +1243,24 @@
         <v>18</v>
       </c>
       <c r="D48" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="E48" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="E48" s="6" t="s">
-        <v>77</v>
-      </c>
       <c r="F48" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>32</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D49" s="9" t="s">
         <v>18</v>
@@ -1239,18 +1269,18 @@
         <v>18</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D50" s="9" t="s">
         <v>22</v>
@@ -1259,18 +1289,18 @@
         <v>22</v>
       </c>
       <c r="F50" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D51" s="9" t="s">
         <v>22</v>
@@ -1279,7 +1309,7 @@
         <v>22</v>
       </c>
       <c r="F51" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -1388,13 +1418,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B29:B51">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",B29)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",B29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Partial">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Partial">
       <formula>NOT(ISERROR(SEARCH("Partial",B29)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>